<commit_message>
- Modified budget - Added budget justification - Project description now includes more complete atmospheric blocking and atmospheric river sections
</commit_message>
<xml_diff>
--- a/Ullrich-NASAClimateIndicators-ZarzyckiBudget.xlsx
+++ b/Ullrich-NASAClimateIndicators-ZarzyckiBudget.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23300" windowHeight="19060" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="7620" yWindow="0" windowWidth="23300" windowHeight="19060" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" state="hidden" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="194">
   <si>
     <t>Project Information</t>
   </si>
@@ -824,31 +824,16 @@
     <t>Non-Federal</t>
   </si>
   <si>
-    <t>R. Grotjahn (PI)</t>
-  </si>
-  <si>
-    <t>P. Ullrich (co-PI)</t>
-  </si>
-  <si>
-    <t>TBN (GSR IV)</t>
-  </si>
-  <si>
-    <t>50 TB external harddrives for storing modeling data generated for this project</t>
-  </si>
-  <si>
     <t>Ullrich, Grotjahn</t>
   </si>
   <si>
     <t>TempestExtremes: Indicators of change in the characteristics of extreme weather</t>
   </si>
   <si>
-    <t>Int'l Assoc. of Meteorology and Atmospheric Sciences (IAMAS) Cape Town South Africa conference</t>
+    <t>Domestic conference</t>
   </si>
   <si>
-    <t>American Meteorological society (AMS) climate Variations conference</t>
-  </si>
-  <si>
-    <t>American Geophysical Union (AGU) fall meeting San Francisco (x2)</t>
+    <t>Travel to UC Davis</t>
   </si>
 </sst>
 </file>
@@ -7326,15 +7311,15 @@
       </c>
       <c r="C157" s="43">
         <f ca="1">Request!N60+Request!N84+Request!N96+Request!N126+SUM(Request!N136:N140)+SUM(Request!N151:N158)+Worksheet!C136</f>
-        <v>90875</v>
+        <v>2650</v>
       </c>
       <c r="D157" s="43">
         <f ca="1">IF(D4="",0,(Request!O60+Request!O84+Request!O96+Request!O126+SUM(Request!O136:O140)+SUM(Request!O151:O158)+Worksheet!D136))</f>
-        <v>94454</v>
+        <v>2650</v>
       </c>
       <c r="E157" s="43">
         <f ca="1">IF(E4="",0,(Request!P60+Request!P84+Request!P96+Request!P126+SUM(Request!P136:P140)+SUM(Request!P151:P158)+Worksheet!E136))</f>
-        <v>95098</v>
+        <v>2650</v>
       </c>
       <c r="F157" s="43">
         <f>IF(F4="",0,(Request!Q60+Request!Q84+Request!Q96+Request!Q126+SUM(Request!Q136:Q140)+SUM(Request!Q151:Q158)+Worksheet!F136))</f>
@@ -7346,7 +7331,7 @@
       </c>
       <c r="H157" s="45">
         <f ca="1">SUM(C157:G157)</f>
-        <v>280427</v>
+        <v>7950</v>
       </c>
       <c r="I157" s="23"/>
       <c r="J157" s="23"/>
@@ -7367,15 +7352,15 @@
       </c>
       <c r="C158" s="45">
         <f ca="1">Request!N161-Request!N114+Worksheet!C154</f>
-        <v>104521</v>
+        <v>2650</v>
       </c>
       <c r="D158" s="45">
         <f ca="1">IF(D4="",0,(Request!O161-Request!O114+Worksheet!D154))</f>
-        <v>109464.6</v>
+        <v>2650</v>
       </c>
       <c r="E158" s="45">
         <f ca="1">IF(E4="",0,(Request!P161-Request!P114+Worksheet!E154))</f>
-        <v>111609.66</v>
+        <v>2650</v>
       </c>
       <c r="F158" s="45">
         <f>IF(F4="",0,(Request!Q161-Request!Q114+Worksheet!F154))</f>
@@ -7387,7 +7372,7 @@
       </c>
       <c r="H158" s="45">
         <f ca="1">SUM(C158:G158)</f>
-        <v>325595.26</v>
+        <v>7950</v>
       </c>
       <c r="I158" s="23"/>
       <c r="J158" s="23"/>
@@ -7408,15 +7393,15 @@
       </c>
       <c r="C159" s="43">
         <f ca="1">ROUND((Request!N161-Request!N114+Worksheet!C154)/(1-Request!$L$164),0)</f>
-        <v>130651</v>
+        <v>3313</v>
       </c>
       <c r="D159" s="43">
         <f ca="1">IF(D4="",0,(ROUND((Request!O161-Request!O114+Worksheet!D154)/(1-Request!$L$164),0)))</f>
-        <v>136831</v>
+        <v>3313</v>
       </c>
       <c r="E159" s="43">
         <f ca="1">IF(E4="",0,(ROUND((Request!P161-Request!P114+Worksheet!E154)/(1-Request!$L$164),0)))</f>
-        <v>139512</v>
+        <v>3313</v>
       </c>
       <c r="F159" s="43">
         <f>IF(F4="",0,(ROUND((Request!Q161-Request!Q114+Worksheet!F154)/(1-Request!$L$164),0)))</f>
@@ -7428,7 +7413,7 @@
       </c>
       <c r="H159" s="45">
         <f ca="1">SUM(C159:G159)</f>
-        <v>406994</v>
+        <v>9939</v>
       </c>
       <c r="I159" s="23"/>
       <c r="J159" s="23"/>
@@ -7730,9 +7715,9 @@
       </c>
     </row>
     <row r="171" spans="1:19">
-      <c r="A171" s="42" t="str">
+      <c r="A171" s="42">
         <f>Request!B7</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="B171" s="4">
         <f>IF($G171&lt;Worksheet!C$5,$G171,Worksheet!C$5)</f>
@@ -7780,9 +7765,9 @@
       </c>
     </row>
     <row r="172" spans="1:19">
-      <c r="A172" s="42" t="str">
+      <c r="A172" s="42">
         <f>Request!B8</f>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="B172" s="4">
         <f>IF($G172&lt;Worksheet!C$5,$G172,Worksheet!C$5)</f>
@@ -7830,9 +7815,9 @@
       </c>
     </row>
     <row r="173" spans="1:19">
-      <c r="A173" s="42" t="str">
+      <c r="A173" s="42">
         <f>Request!B9</f>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B173" s="4">
         <f>IF($G173&lt;Worksheet!C$5,$G173,Worksheet!C$5)</f>
@@ -7880,9 +7865,9 @@
       </c>
     </row>
     <row r="174" spans="1:19">
-      <c r="A174" s="42" t="str">
+      <c r="A174" s="42">
         <f>Request!B10</f>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B174" s="4">
         <f>IF($G174&lt;Worksheet!C$5,$G174,Worksheet!C$5)</f>
@@ -9291,9 +9276,9 @@
       <c r="K211" s="219"/>
     </row>
     <row r="212" spans="1:12">
-      <c r="A212" s="93" t="str">
+      <c r="A212" s="93">
         <f t="shared" ref="A212:A235" si="57">A171</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="B212" s="4">
         <f>IF(L212="A",IF(H171&lt;$E$198,H171,$E$198),IF(L212="B",IF(H171&lt;$E$204,H171,$E$204),IF(L212="C",IF(H171&lt;$E$206,H171,$E$206),IF(L212="D",0))))</f>
@@ -9341,9 +9326,9 @@
       </c>
     </row>
     <row r="213" spans="1:12">
-      <c r="A213" s="94" t="str">
+      <c r="A213" s="94">
         <f t="shared" si="57"/>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="B213" s="4">
         <f t="shared" ref="B213:B235" si="63">IF(L213="A",IF(H172&lt;$E$198,H172,$E$198),IF(L213="B",IF(H172&lt;$E$204,H172,$E$204),IF(L213="C",IF(H172&lt;$E$206,H172,$E$206),IF(L213="D",0))))</f>
@@ -9391,9 +9376,9 @@
       </c>
     </row>
     <row r="214" spans="1:12">
-      <c r="A214" s="94" t="str">
+      <c r="A214" s="94">
         <f t="shared" si="57"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B214" s="4">
         <f t="shared" si="63"/>
@@ -9441,9 +9426,9 @@
       </c>
     </row>
     <row r="215" spans="1:12">
-      <c r="A215" s="94" t="str">
+      <c r="A215" s="94">
         <f t="shared" si="57"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B215" s="4">
         <f t="shared" si="63"/>
@@ -10566,9 +10551,9 @@
       </c>
     </row>
     <row r="242" spans="1:11">
-      <c r="A242" s="93" t="str">
+      <c r="A242" s="93">
         <f>A212</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="B242" s="4">
         <f>B212</f>
@@ -10612,9 +10597,9 @@
       </c>
     </row>
     <row r="243" spans="1:11">
-      <c r="A243" s="93" t="str">
+      <c r="A243" s="93">
         <f t="shared" ref="A243:K265" si="70">A213</f>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="B243" s="4">
         <f t="shared" si="70"/>
@@ -10658,9 +10643,9 @@
       </c>
     </row>
     <row r="244" spans="1:11">
-      <c r="A244" s="93" t="str">
-        <f t="shared" si="70"/>
-        <v>TBN (GSR IV)</v>
+      <c r="A244" s="93">
+        <f t="shared" si="70"/>
+        <v>0</v>
       </c>
       <c r="B244" s="4">
         <f t="shared" si="70"/>
@@ -10704,9 +10689,9 @@
       </c>
     </row>
     <row r="245" spans="1:11">
-      <c r="A245" s="93" t="str">
-        <f t="shared" si="70"/>
-        <v>TBN (GSR IV)</v>
+      <c r="A245" s="93">
+        <f t="shared" si="70"/>
+        <v>0</v>
       </c>
       <c r="B245" s="4">
         <f t="shared" si="70"/>
@@ -11698,9 +11683,9 @@
       <c r="K268" s="212"/>
     </row>
     <row r="269" spans="1:11">
-      <c r="A269" s="101" t="str">
+      <c r="A269" s="101">
         <f>A242</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="B269" s="215" t="str">
         <f>IF(B$241=C$241,B$241*100,IF(C242=0,B$241*100,IF(B242=0,C$241*100,B$241*100&amp;"/"&amp;C$241*100)))</f>
@@ -11729,9 +11714,9 @@
       <c r="K269" s="214"/>
     </row>
     <row r="270" spans="1:11">
-      <c r="A270" s="101" t="str">
+      <c r="A270" s="101">
         <f t="shared" ref="A270:A292" si="74">A243</f>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="B270" s="215" t="str">
         <f t="shared" ref="B270:B292" si="75">IF(B$241=C$241,B$241*100,IF(C243=0,B$241*100,IF(B243=0,C$241*100,B$241*100&amp;"/"&amp;C$241*100)))</f>
@@ -11760,9 +11745,9 @@
       <c r="K270" s="214"/>
     </row>
     <row r="271" spans="1:11">
-      <c r="A271" s="101" t="str">
+      <c r="A271" s="101">
         <f t="shared" si="74"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B271" s="215">
         <f t="shared" si="75"/>
@@ -11791,9 +11776,9 @@
       <c r="K271" s="214"/>
     </row>
     <row r="272" spans="1:11">
-      <c r="A272" s="101" t="str">
+      <c r="A272" s="101">
         <f t="shared" si="74"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B272" s="215">
         <f t="shared" si="75"/>
@@ -12457,23 +12442,23 @@
       <c r="K294" s="212"/>
     </row>
     <row r="295" spans="1:12">
-      <c r="A295" s="101" t="str">
+      <c r="A295" s="101">
         <f>A269</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="B295" s="210">
         <f ca="1">ROUND(Request!N7/Worksheet!H171*Worksheet!B242*Worksheet!$B$241+Request!N7/Worksheet!H171*Worksheet!C242*Worksheet!C241,0)</f>
-        <v>2478</v>
+        <v>0</v>
       </c>
       <c r="C295" s="211"/>
       <c r="D295" s="210">
         <f ca="1">ROUND(Request!O7/(D242+E242)*Worksheet!D242*Worksheet!D$241+Request!O7/(D242+E242)*Worksheet!E242*Worksheet!E$241,0)</f>
-        <v>2675</v>
+        <v>0</v>
       </c>
       <c r="E295" s="211"/>
       <c r="F295" s="210">
         <f ca="1">ROUND(Request!P7/(F242+G242)*Worksheet!F242*Worksheet!F$241+Request!P7/(F242+G242)*Worksheet!G242*Worksheet!G$241,0)</f>
-        <v>2836</v>
+        <v>0</v>
       </c>
       <c r="G295" s="211"/>
       <c r="H295" s="210" t="e">
@@ -12488,23 +12473,23 @@
       <c r="K295" s="211"/>
     </row>
     <row r="296" spans="1:12">
-      <c r="A296" s="101" t="str">
+      <c r="A296" s="101">
         <f t="shared" ref="A296:A318" si="80">A270</f>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="B296" s="210">
         <f ca="1">ROUND(Request!N8/Worksheet!H172*Worksheet!B243*Worksheet!$B$241+Request!N8/Worksheet!H172*Worksheet!C243*Worksheet!$C$241,0)</f>
-        <v>1421</v>
+        <v>0</v>
       </c>
       <c r="C296" s="211"/>
       <c r="D296" s="210">
         <f ca="1">ROUND(Request!O8/(D243+E243)*Worksheet!D243*Worksheet!D$241+Request!O8/(D243+E243)*Worksheet!E243*Worksheet!E$241,0)</f>
-        <v>1534</v>
+        <v>0</v>
       </c>
       <c r="E296" s="211"/>
       <c r="F296" s="210">
         <f ca="1">ROUND(Request!P8/(F243+G243)*Worksheet!F243*Worksheet!F$241+Request!P8/(F243+G243)*Worksheet!G243*Worksheet!G$241,0)</f>
-        <v>1626</v>
+        <v>0</v>
       </c>
       <c r="G296" s="211"/>
       <c r="H296" s="210" t="e">
@@ -12519,23 +12504,23 @@
       <c r="K296" s="211"/>
     </row>
     <row r="297" spans="1:12">
-      <c r="A297" s="101" t="str">
+      <c r="A297" s="101">
         <f t="shared" si="80"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B297" s="210">
         <f ca="1">ROUND(Request!N9/Worksheet!H173*Worksheet!B244*Worksheet!$B$241+Request!N9/Worksheet!H173*Worksheet!C244*Worksheet!$C$241,0)</f>
-        <v>5165</v>
+        <v>0</v>
       </c>
       <c r="C297" s="211"/>
       <c r="D297" s="210">
         <f ca="1">ROUND(Request!O9/(D244+E244)*Worksheet!D244*Worksheet!D$241+Request!O9/(D244+E244)*Worksheet!E244*Worksheet!E$241,0)</f>
-        <v>5468</v>
+        <v>0</v>
       </c>
       <c r="E297" s="211"/>
       <c r="F297" s="210">
         <f ca="1">ROUND(Request!P9/(F244+G244)*Worksheet!F244*Worksheet!F$241+Request!P9/(F244+G244)*Worksheet!G244*Worksheet!G$241,0)</f>
-        <v>5814</v>
+        <v>0</v>
       </c>
       <c r="G297" s="211"/>
       <c r="H297" s="210" t="e">
@@ -12550,23 +12535,23 @@
       <c r="K297" s="211"/>
     </row>
     <row r="298" spans="1:12">
-      <c r="A298" s="101" t="str">
+      <c r="A298" s="101">
         <f t="shared" si="80"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="B298" s="210">
         <f ca="1">ROUND(Request!N10/Worksheet!H174*Worksheet!B245*Worksheet!$B$241+Request!N10/Worksheet!H174*Worksheet!C245*Worksheet!$C$241,0)</f>
-        <v>5165</v>
+        <v>0</v>
       </c>
       <c r="C298" s="211"/>
       <c r="D298" s="210">
         <f ca="1">ROUND(Request!O10/(D245+E245)*Worksheet!D245*Worksheet!D$241+Request!O10/(D245+E245)*Worksheet!E245*Worksheet!E$241,0)</f>
-        <v>5468</v>
+        <v>0</v>
       </c>
       <c r="E298" s="211"/>
       <c r="F298" s="210">
         <f ca="1">ROUND(Request!P10/(F245+G245)*Worksheet!F245*Worksheet!F$241+Request!P10/(F245+G245)*Worksheet!G245*Worksheet!G$241,0)</f>
-        <v>5814</v>
+        <v>0</v>
       </c>
       <c r="G298" s="211"/>
       <c r="H298" s="210" t="e">
@@ -13534,8 +13519,8 @@
   </sheetPr>
   <dimension ref="A1:X170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:M31"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -13576,7 +13561,7 @@
       </c>
       <c r="E1" s="242"/>
       <c r="F1" s="280" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G1" s="276"/>
       <c r="H1" s="276"/>
@@ -13605,7 +13590,7 @@
       </c>
       <c r="E2" s="242"/>
       <c r="F2" s="280" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G2" s="276"/>
       <c r="H2" s="276"/>
@@ -13761,13 +13746,11 @@
       <c r="A7" s="162">
         <v>1</v>
       </c>
-      <c r="B7" s="262" t="s">
-        <v>190</v>
-      </c>
+      <c r="B7" s="262"/>
       <c r="C7" s="262"/>
       <c r="D7" s="273"/>
       <c r="E7" s="183">
-        <v>165709.09</v>
+        <v>0</v>
       </c>
       <c r="F7" s="105">
         <v>8.3330000000000001E-2</v>
@@ -13787,15 +13770,15 @@
       </c>
       <c r="N7" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M7)^Worksheet!$B$20*Worksheet!$C$9+(1+$M7)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E7*Request!$F7,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E7*$F7/12*Worksheet!$C$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^Worksheet!$B$20*Worksheet!$C$9+(1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E7*Request!$F7,0),ROUND($E7*$F7/12*Worksheet!$C$5,0))))))</f>
-        <v>14294</v>
+        <v>0</v>
       </c>
       <c r="O7" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M7)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$M7)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E7*Request!$G7,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E7*$G7*(1+M7)/12*Worksheet!$D$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E7*Request!$G7,0),ROUND($E7*$G7*(1+$S$4)/12*Worksheet!$D$5,0))))))</f>
-        <v>14723</v>
+        <v>0</v>
       </c>
       <c r="P7" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M7)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$M7)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E7*Request!H7,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E7*H7*((1+$M7)^2)/12*Worksheet!$E$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E7*Request!H7,0),ROUND($E7*H7*((1+$S$4)^2)/12*Worksheet!$E$5,0))))))</f>
-        <v>15164</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M7)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$M7)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E7*Request!$I7,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E7*$I7*((1+$M7)^3)/12*Worksheet!$F$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$S$4)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E7*Request!$I7,0),ROUND($E7*$I7*((1+$S$4)^3)/12*Worksheet!$F$5,0))))))</f>
@@ -13807,7 +13790,7 @@
       </c>
       <c r="S7" s="155">
         <f ca="1">SUM(N7:R7)</f>
-        <v>44181</v>
+        <v>0</v>
       </c>
       <c r="T7" s="61"/>
       <c r="U7" s="61"/>
@@ -13819,13 +13802,11 @@
       <c r="A8" s="162">
         <v>2</v>
       </c>
-      <c r="B8" s="262" t="s">
-        <v>191</v>
-      </c>
+      <c r="B8" s="262"/>
       <c r="C8" s="262"/>
       <c r="D8" s="175"/>
       <c r="E8" s="183">
-        <v>95020.36</v>
+        <v>0</v>
       </c>
       <c r="F8" s="105">
         <v>8.3330000000000001E-2</v>
@@ -13845,15 +13826,15 @@
       </c>
       <c r="N8" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M8)^Worksheet!$B$20*Worksheet!$C$9+(1+$M8)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E8*Request!$F8,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND(E8*F8/12*Worksheet!$C$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^Worksheet!$B$20*Worksheet!$C$9+(1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E8*Request!$F8,0),ROUND($E8*$F8/12*Worksheet!$C$5,0))))))</f>
-        <v>8196</v>
+        <v>0</v>
       </c>
       <c r="O8" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M8)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$M8)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E8*Request!$G8,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E8*$G8*(1+M8)/12*Worksheet!$D$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E8*Request!$G8,0),ROUND($E8*$G8*(1+$S$4)/12*Worksheet!$D$5,0))))))</f>
-        <v>8442</v>
+        <v>0</v>
       </c>
       <c r="P8" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M8)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$M8)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E8*Request!H8,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E8*H8*((1+$M8)^2)/12*Worksheet!$E$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E8*Request!H8,0),ROUND($E8*H8*((1+$S$4)^2)/12*Worksheet!$E$5,0))))))</f>
-        <v>8696</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M8)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$M8)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E8*Request!$I8,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E8*$I8*((1+$M8)^3)/12*Worksheet!$F$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$S$4)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E8*Request!$I8,0),ROUND($E8*$I8*((1+$S$4)^3)/12*Worksheet!$F$5,0))))))</f>
@@ -13865,7 +13846,7 @@
       </c>
       <c r="S8" s="155">
         <f t="shared" ref="S8:S30" ca="1" si="0">SUM(N8:R8)</f>
-        <v>25334</v>
+        <v>0</v>
       </c>
       <c r="T8" s="61"/>
       <c r="U8" s="61"/>
@@ -13877,13 +13858,11 @@
       <c r="A9" s="162">
         <v>3</v>
       </c>
-      <c r="B9" s="262" t="s">
-        <v>192</v>
-      </c>
+      <c r="B9" s="262"/>
       <c r="C9" s="262"/>
       <c r="D9" s="273"/>
       <c r="E9" s="183">
-        <v>45300</v>
+        <v>0</v>
       </c>
       <c r="F9" s="105">
         <v>0.61192999999999997</v>
@@ -13903,15 +13882,15 @@
       </c>
       <c r="N9" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M9)^Worksheet!$B$20*Worksheet!$C$9+(1+$M9)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E9*Request!$F9,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND(E9*F9/12*Worksheet!$C$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^Worksheet!$B$20*Worksheet!$C$9+(1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E9*Request!$F9,0),ROUND($E9*$F9/12*Worksheet!$C$5,0))))))</f>
-        <v>28695</v>
+        <v>0</v>
       </c>
       <c r="O9" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M9)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$M9)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E9*Request!$G9,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E9*$G9*(1+M9)/12*Worksheet!$D$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E9*Request!$G9,0),ROUND($E9*$G9*(1+$S$4)/12*Worksheet!$D$5,0))))))</f>
-        <v>29556</v>
+        <v>0</v>
       </c>
       <c r="P9" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M9)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$M9)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E9*Request!H9,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E9*H9*((1+$M9)^2)/12*Worksheet!$E$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E9*Request!H9,0),ROUND($E9*H9*((1+$S$4)^2)/12*Worksheet!$E$5,0))))))</f>
-        <v>30442</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M9)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$M9)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E9*Request!$I9,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E9*$I9*((1+$M9)^3)/12*Worksheet!$F$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$S$4)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E9*Request!$I9,0),ROUND($E9*$I9*((1+$S$4)^3)/12*Worksheet!$F$5,0))))))</f>
@@ -13923,7 +13902,7 @@
       </c>
       <c r="S9" s="155">
         <f t="shared" ca="1" si="0"/>
-        <v>88693</v>
+        <v>0</v>
       </c>
       <c r="T9" s="61"/>
       <c r="U9" s="61"/>
@@ -13935,13 +13914,11 @@
       <c r="A10" s="162">
         <v>4</v>
       </c>
-      <c r="B10" s="262" t="s">
-        <v>192</v>
-      </c>
+      <c r="B10" s="262"/>
       <c r="C10" s="262"/>
       <c r="D10" s="273"/>
       <c r="E10" s="183">
-        <v>45300</v>
+        <v>0</v>
       </c>
       <c r="F10" s="105">
         <v>0.61192999999999997</v>
@@ -13961,15 +13938,15 @@
       </c>
       <c r="N10" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M10)^Worksheet!$B$20*Worksheet!$C$9+(1+$M10)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E10*Request!$F10,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND(E10*F10/12*Worksheet!$C$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^Worksheet!$B$20*Worksheet!$C$9+(1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$C$10)/12*Request!$E10*Request!$F10,0),ROUND($E10*$F10/12*Worksheet!$C$5,0))))))</f>
-        <v>28695</v>
+        <v>0</v>
       </c>
       <c r="O10" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M10)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$M10)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E10*Request!$G10,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E10*$G10*(1+M10)/12*Worksheet!$D$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+1)*Worksheet!$D$9+(1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$D$10)/12*Request!$E10*Request!$G10,0),ROUND($E10*$G10*(1+$S$4)/12*Worksheet!$D$5,0))))))</f>
-        <v>29556</v>
+        <v>0</v>
       </c>
       <c r="P10" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M10)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$M10)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E10*Request!H10,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E10*H10*((1+$M10)^2)/12*Worksheet!$E$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+2)*Worksheet!$E$9+(1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$E$10)/12*Request!$E10*Request!H10,0),ROUND($E10*H10*((1+$S$4)^2)/12*Worksheet!$E$5,0))))))</f>
-        <v>30442</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="80">
         <f ca="1">IF(AND($S$4="Multi",$R$4="FY"),ROUND(((1+$M10)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$M10)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E10*Request!$I10,0),(IF(AND($S$4="Multi",$R$4="PY"),ROUND($E10*$I10*((1+$M10)^3)/12*Worksheet!$F$5,0),(IF(AND($S$4&lt;&gt;"Multi",$R$4="FY"),ROUND(((1+$S$4)^(Worksheet!$B$20+3)*Worksheet!$F$9+(1+$S$4)^(Worksheet!$B$20+4)*Worksheet!$F$10)/12*Request!$E10*Request!$I10,0),ROUND($E10*$I10*((1+$S$4)^3)/12*Worksheet!$F$5,0))))))</f>
@@ -13981,7 +13958,7 @@
       </c>
       <c r="S10" s="155">
         <f t="shared" ca="1" si="0"/>
-        <v>88693</v>
+        <v>0</v>
       </c>
       <c r="T10" s="61"/>
       <c r="U10" s="61"/>
@@ -14967,15 +14944,15 @@
       <c r="M31" s="233"/>
       <c r="N31" s="158">
         <f ca="1">SUM(N7:N30)</f>
-        <v>79880</v>
+        <v>0</v>
       </c>
       <c r="O31" s="158">
         <f ca="1">SUM(O7:O30)</f>
-        <v>82277</v>
+        <v>0</v>
       </c>
       <c r="P31" s="158">
         <f t="shared" ref="P31:Q31" ca="1" si="1">SUM(P7:P30)</f>
-        <v>84744</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="158">
         <f t="shared" ca="1" si="1"/>
@@ -14987,7 +14964,7 @@
       </c>
       <c r="S31" s="158">
         <f ca="1">SUM(S7:S30)</f>
-        <v>246901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="9" customHeight="1">
@@ -15096,9 +15073,9 @@
       <c r="A35" s="162">
         <v>1</v>
       </c>
-      <c r="B35" s="262" t="str">
+      <c r="B35" s="262">
         <f t="shared" ref="B35:B58" si="2">B7</f>
-        <v>R. Grotjahn (PI)</v>
+        <v>0</v>
       </c>
       <c r="C35" s="263"/>
       <c r="D35" s="179" t="s">
@@ -15124,15 +15101,15 @@
       <c r="M35" s="261"/>
       <c r="N35" s="80">
         <f ca="1">IF(AND($D35="F-SMRA",N7=0),0,IF(AND($D35="F-SMRB",N7=0),0,IF(AND($D35="F-SMRC",N7=0),0,IF($D35=Worksheet!$A$68,Worksheet!B295,IF($D35=Worksheet!$A$69,Worksheet!B295,IF($D35=Worksheet!$A$70,Worksheet!B295,ROUND((Request!N7/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D35=Worksheet!$A$47,Worksheet!B$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!B$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!B$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!B$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!B$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!B$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!B$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!B$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!B$55))))))))))),0)+ROUND(N7/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D35=Worksheet!$A$47,Worksheet!C$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!C$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!C$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!C$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!C$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!C$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!C$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!C$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!C$55)))))))))),0)))))))</f>
-        <v>2478</v>
+        <v>0</v>
       </c>
       <c r="O35" s="80">
         <f ca="1">IF(AND($D35="F-SMRA",O7=0),0,IF(AND($D35="F-SMRB",O7=0),0,IF(AND($D35="F-SMRC",O7=0),0,IF($D35=Worksheet!$A$68,Worksheet!D295,IF($D35=Worksheet!$A$69,Worksheet!D295,IF($D35=Worksheet!$A$70,Worksheet!D295,ROUND((Request!O7/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D35=Worksheet!$A$47,Worksheet!D$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!D$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!D$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!D$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!D$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!D$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!D$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!D$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!D$55))))))))))),0)+ROUND(O7/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D35=Worksheet!$A$47,Worksheet!E$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!E$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!E$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!E$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!E$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!E$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!E$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!E$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!E$55)))))))))),0)))))))</f>
-        <v>2675</v>
+        <v>0</v>
       </c>
       <c r="P35" s="80">
         <f ca="1">IF(AND($D35="F-SMRA",P7=0),0,IF(AND($D35="F-SMRB",P7=0),0,IF(AND($D35="F-SMRC",P7=0),0,IF($D35=Worksheet!$A$68,Worksheet!F295,IF($D35=Worksheet!$A$69,Worksheet!F295,IF($D35=Worksheet!$A$70,Worksheet!F295,ROUND((Request!P7/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D35=Worksheet!$A$47,Worksheet!F$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!F$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!F$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!F$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!F$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!F$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!F$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!F$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!F$55))))))))))),0)+ROUND(P7/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D35=Worksheet!$A$47,Worksheet!G$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!G$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!G$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!G$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!G$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!G$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!G$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!G$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!G$55)))))))))),0)))))))</f>
-        <v>2836</v>
+        <v>0</v>
       </c>
       <c r="Q35" s="80">
         <f ca="1">IF(AND($D35="F-SMRA",Q7=0),0,IF(AND($D35="F-SMRB",Q7=0),0,IF(AND($D35="F-SMRC",Q7=0),0,IF($D35=Worksheet!$A$68,Worksheet!H295,IF($D35=Worksheet!$A$69,Worksheet!H295,IF($D35=Worksheet!$A$70,Worksheet!H295,ROUND((Request!Q7/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D35=Worksheet!$A$47,Worksheet!H$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!H$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!H$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!H$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!H$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!H$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!H$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!H$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!H$55))))))))))),0)+ROUND(Q7/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D35=Worksheet!$A$47,Worksheet!I$47,IF(Request!$D35=Worksheet!$A$48,Worksheet!I$48,IF(Request!$D35=Worksheet!$A$49,Worksheet!I$49,IF(Request!$D35=Worksheet!$A$50,Worksheet!I$50,IF(Request!$D35=Worksheet!$A$51,Worksheet!I$51,IF(Request!$D35=Worksheet!$A$52,Worksheet!I$52,IF(Request!$D35=Worksheet!$A$53,Worksheet!I$53,IF(Request!$D35=Worksheet!$A$54,Worksheet!I$54,IF(Request!$D35=Worksheet!$A$55,Worksheet!I$55)))))))))),0)))))))</f>
@@ -15144,7 +15121,7 @@
       </c>
       <c r="S35" s="80">
         <f ca="1">SUM(N35:R35)</f>
-        <v>7989</v>
+        <v>0</v>
       </c>
       <c r="T35" s="65"/>
       <c r="U35" s="65"/>
@@ -15156,9 +15133,9 @@
       <c r="A36" s="162">
         <v>2</v>
       </c>
-      <c r="B36" s="262" t="str">
+      <c r="B36" s="262">
         <f t="shared" si="2"/>
-        <v>P. Ullrich (co-PI)</v>
+        <v>0</v>
       </c>
       <c r="C36" s="263"/>
       <c r="D36" s="179" t="s">
@@ -15184,15 +15161,15 @@
       <c r="M36" s="261"/>
       <c r="N36" s="80">
         <f ca="1">IF(AND(D36="F-SMRA",N8=0),0,IF(AND(D36="F-SMRB",N8=0),0,IF(AND(D36="F-SMRC",N8=0),0,IF($D36=Worksheet!$A$68,Worksheet!B296,IF($D36=Worksheet!$A$69,Worksheet!B296,IF($D36=Worksheet!$A$70,Worksheet!B296,ROUND((Request!N8/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D36=Worksheet!$A$47,Worksheet!B$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!B$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!B$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!B$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!B$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!B$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!B$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!B$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!B$55))))))))))),0)+ROUND(N8/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D36=Worksheet!$A$47,Worksheet!C$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!C$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!C$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!C$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!C$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!C$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!C$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!C$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!C$55)))))))))),0)))))))</f>
-        <v>1421</v>
+        <v>0</v>
       </c>
       <c r="O36" s="80">
         <f ca="1">IF(AND($D36="F-SMRA",O8=0),0,IF(AND($D36="F-SMRB",O8=0),0,IF(AND($D36="F-SMRC",O8=0),0,IF($D36=Worksheet!$A$68,Worksheet!D296,IF($D36=Worksheet!$A$69,Worksheet!D296,IF($D36=Worksheet!$A$70,Worksheet!D296,ROUND((Request!O8/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D36=Worksheet!$A$47,Worksheet!D$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!D$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!D$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!D$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!D$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!D$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!D$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!D$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!D$55))))))))))),0)+ROUND(O8/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D36=Worksheet!$A$47,Worksheet!E$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!E$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!E$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!E$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!E$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!E$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!E$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!E$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!E$55)))))))))),0)))))))</f>
-        <v>1534</v>
+        <v>0</v>
       </c>
       <c r="P36" s="80">
         <f ca="1">IF(AND($D36="F-SMRA",P8=0),0,IF(AND($D36="F-SMRB",P8=0),0,IF(AND($D36="F-SMRC",P8=0),0,IF($D36=Worksheet!$A$68,Worksheet!F296,IF($D36=Worksheet!$A$69,Worksheet!F296,IF($D36=Worksheet!$A$70,Worksheet!F296,ROUND((Request!P8/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D36=Worksheet!$A$47,Worksheet!F$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!F$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!F$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!F$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!F$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!F$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!F$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!F$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!F$55))))))))))),0)+ROUND(P8/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D36=Worksheet!$A$47,Worksheet!G$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!G$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!G$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!G$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!G$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!G$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!G$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!G$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!G$55)))))))))),0)))))))</f>
-        <v>1626</v>
+        <v>0</v>
       </c>
       <c r="Q36" s="80">
         <f ca="1">IF(AND($D36="F-SMRA",Q8=0),0,IF(AND($D36="F-SMRB",Q8=0),0,IF(AND($D36="F-SMRC",Q8=0),0,IF($D36=Worksheet!$A$68,Worksheet!H296,IF($D36=Worksheet!$A$69,Worksheet!H296,IF($D36=Worksheet!$A$70,Worksheet!H296,ROUND((Request!Q8/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D36=Worksheet!$A$47,Worksheet!H$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!H$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!H$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!H$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!H$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!H$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!H$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!H$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!H$55))))))))))),0)+ROUND(Q8/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D36=Worksheet!$A$47,Worksheet!I$47,IF(Request!$D36=Worksheet!$A$48,Worksheet!I$48,IF(Request!$D36=Worksheet!$A$49,Worksheet!I$49,IF(Request!$D36=Worksheet!$A$50,Worksheet!I$50,IF(Request!$D36=Worksheet!$A$51,Worksheet!I$51,IF(Request!$D36=Worksheet!$A$52,Worksheet!I$52,IF(Request!$D36=Worksheet!$A$53,Worksheet!I$53,IF(Request!$D36=Worksheet!$A$54,Worksheet!I$54,IF(Request!$D36=Worksheet!$A$55,Worksheet!I$55)))))))))),0)))))))</f>
@@ -15204,7 +15181,7 @@
       </c>
       <c r="S36" s="80">
         <f t="shared" ref="S36:S58" ca="1" si="3">SUM(N36:R36)</f>
-        <v>4581</v>
+        <v>0</v>
       </c>
       <c r="T36" s="65"/>
       <c r="U36" s="65"/>
@@ -15216,9 +15193,9 @@
       <c r="A37" s="162">
         <v>3</v>
       </c>
-      <c r="B37" s="262" t="str">
+      <c r="B37" s="262">
         <f t="shared" si="2"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="C37" s="263"/>
       <c r="D37" s="179" t="s">
@@ -15250,15 +15227,15 @@
       <c r="M37" s="261"/>
       <c r="N37" s="80">
         <f ca="1">IF(AND(D37="F-SMRA",N9=0),0,IF(AND(D37="F-SMRB",N9=0),0,IF(AND(D37="F-SMRC",N9=0),0,IF($D37=Worksheet!$A$68,Worksheet!B297,IF($D37=Worksheet!$A$69,Worksheet!B297,IF($D37=Worksheet!$A$70,Worksheet!B297,ROUND((Request!N9/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D37=Worksheet!$A$47,Worksheet!B$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!B$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!B$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!B$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!B$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!B$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!B$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!B$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!B$55))))))))))),0)+ROUND(N9/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D37=Worksheet!$A$47,Worksheet!C$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!C$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!C$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!C$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!C$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!C$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!C$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!C$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!C$55)))))))))),0)))))))</f>
-        <v>373</v>
+        <v>0</v>
       </c>
       <c r="O37" s="80">
         <f ca="1">IF(AND($D37="F-SMRA",O9=0),0,IF(AND($D37="F-SMRB",O9=0),0,IF(AND($D37="F-SMRC",O9=0),0,IF($D37=Worksheet!$A$68,Worksheet!D297,IF($D37=Worksheet!$A$69,Worksheet!D297,IF($D37=Worksheet!$A$70,Worksheet!D297,ROUND((Request!O9/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D37=Worksheet!$A$47,Worksheet!D$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!D$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!D$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!D$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!D$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!D$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!D$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!D$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!D$55))))))))))),0)+ROUND(O9/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D37=Worksheet!$A$47,Worksheet!E$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!E$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!E$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!E$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!E$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!E$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!E$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!E$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!E$55)))))))))),0)))))))</f>
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="P37" s="80">
         <f ca="1">IF(AND($D37="F-SMRA",P9=0),0,IF(AND($D37="F-SMRB",P9=0),0,IF(AND($D37="F-SMRC",P9=0),0,IF($D37=Worksheet!$A$68,Worksheet!F297,IF($D37=Worksheet!$A$69,Worksheet!F297,IF($D37=Worksheet!$A$70,Worksheet!F297,ROUND((Request!P9/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D37=Worksheet!$A$47,Worksheet!F$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!F$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!F$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!F$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!F$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!F$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!F$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!F$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!F$55))))))))))),0)+ROUND(P9/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D37=Worksheet!$A$47,Worksheet!G$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!G$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!G$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!G$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!G$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!G$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!G$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!G$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!G$55)))))))))),0)))))))</f>
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="Q37" s="80">
         <f ca="1">IF(AND($D37="F-SMRA",Q9=0),0,IF(AND($D37="F-SMRB",Q9=0),0,IF(AND($D37="F-SMRC",Q9=0),0,IF($D37=Worksheet!$A$68,Worksheet!H297,IF($D37=Worksheet!$A$69,Worksheet!H297,IF($D37=Worksheet!$A$70,Worksheet!H297,ROUND((Request!Q9/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D37=Worksheet!$A$47,Worksheet!H$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!H$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!H$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!H$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!H$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!H$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!H$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!H$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!H$55))))))))))),0)+ROUND(Q9/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D37=Worksheet!$A$47,Worksheet!I$47,IF(Request!$D37=Worksheet!$A$48,Worksheet!I$48,IF(Request!$D37=Worksheet!$A$49,Worksheet!I$49,IF(Request!$D37=Worksheet!$A$50,Worksheet!I$50,IF(Request!$D37=Worksheet!$A$51,Worksheet!I$51,IF(Request!$D37=Worksheet!$A$52,Worksheet!I$52,IF(Request!$D37=Worksheet!$A$53,Worksheet!I$53,IF(Request!$D37=Worksheet!$A$54,Worksheet!I$54,IF(Request!$D37=Worksheet!$A$55,Worksheet!I$55)))))))))),0)))))))</f>
@@ -15270,7 +15247,7 @@
       </c>
       <c r="S37" s="80">
         <f t="shared" ca="1" si="3"/>
-        <v>1153</v>
+        <v>0</v>
       </c>
       <c r="T37" s="65"/>
       <c r="U37" s="65"/>
@@ -15282,9 +15259,9 @@
       <c r="A38" s="162">
         <v>4</v>
       </c>
-      <c r="B38" s="262" t="str">
+      <c r="B38" s="262">
         <f t="shared" si="2"/>
-        <v>TBN (GSR IV)</v>
+        <v>0</v>
       </c>
       <c r="C38" s="263"/>
       <c r="D38" s="179" t="s">
@@ -15316,15 +15293,15 @@
       <c r="M38" s="261"/>
       <c r="N38" s="80">
         <f ca="1">IF(AND(D38="F-SMRA",N10=0),0,IF(AND(D38="F-SMRB",N10=0),0,IF(AND(D38="F-SMRC",N10=0),0,IF($D38=Worksheet!$A$68,Worksheet!B298,IF($D38=Worksheet!$A$69,Worksheet!B298,IF($D38=Worksheet!$A$70,Worksheet!B298,ROUND((Request!N10/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D38=Worksheet!$A$47,Worksheet!B$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!B$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!B$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!B$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!B$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!B$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!B$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!B$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!B$55))))))))))),0)+ROUND(N10/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D38=Worksheet!$A$47,Worksheet!C$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!C$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!C$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!C$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!C$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!C$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!C$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!C$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!C$55)))))))))),0)))))))</f>
-        <v>373</v>
+        <v>0</v>
       </c>
       <c r="O38" s="80">
         <f ca="1">IF(AND($D38="F-SMRA",O10=0),0,IF(AND($D38="F-SMRB",O10=0),0,IF(AND($D38="F-SMRC",O10=0),0,IF($D38=Worksheet!$A$68,Worksheet!D298,IF($D38=Worksheet!$A$69,Worksheet!D298,IF($D38=Worksheet!$A$70,Worksheet!D298,ROUND((Request!O10/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D38=Worksheet!$A$47,Worksheet!D$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!D$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!D$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!D$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!D$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!D$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!D$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!D$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!D$55))))))))))),0)+ROUND(O10/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D38=Worksheet!$A$47,Worksheet!E$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!E$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!E$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!E$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!E$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!E$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!E$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!E$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!E$55)))))))))),0)))))))</f>
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="P38" s="80">
         <f ca="1">IF(AND($D38="F-SMRA",P10=0),0,IF(AND($D38="F-SMRB",P10=0),0,IF(AND($D38="F-SMRC",P10=0),0,IF($D38=Worksheet!$A$68,Worksheet!F298,IF($D38=Worksheet!$A$69,Worksheet!F298,IF($D38=Worksheet!$A$70,Worksheet!F298,ROUND((Request!P10/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D38=Worksheet!$A$47,Worksheet!F$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!F$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!F$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!F$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!F$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!F$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!F$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!F$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!F$55))))))))))),0)+ROUND(P10/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D38=Worksheet!$A$47,Worksheet!G$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!G$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!G$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!G$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!G$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!G$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!G$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!G$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!G$55)))))))))),0)))))))</f>
-        <v>396</v>
+        <v>0</v>
       </c>
       <c r="Q38" s="80">
         <f ca="1">IF(AND($D38="F-SMRA",Q10=0),0,IF(AND($D38="F-SMRB",Q10=0),0,IF(AND($D38="F-SMRC",Q10=0),0,IF($D38=Worksheet!$A$68,Worksheet!H298,IF($D38=Worksheet!$A$69,Worksheet!H298,IF($D38=Worksheet!$A$70,Worksheet!H298,ROUND((Request!Q10/Worksheet!$C$5*Worksheet!$C$9*(IF(Request!$D38=Worksheet!$A$47,Worksheet!H$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!H$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!H$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!H$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!H$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!H$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!H$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!H$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!H$55))))))))))),0)+ROUND(Q10/Worksheet!$C$5*Worksheet!$C$10*(IF(Request!$D38=Worksheet!$A$47,Worksheet!I$47,IF(Request!$D38=Worksheet!$A$48,Worksheet!I$48,IF(Request!$D38=Worksheet!$A$49,Worksheet!I$49,IF(Request!$D38=Worksheet!$A$50,Worksheet!I$50,IF(Request!$D38=Worksheet!$A$51,Worksheet!I$51,IF(Request!$D38=Worksheet!$A$52,Worksheet!I$52,IF(Request!$D38=Worksheet!$A$53,Worksheet!I$53,IF(Request!$D38=Worksheet!$A$54,Worksheet!I$54,IF(Request!$D38=Worksheet!$A$55,Worksheet!I$55)))))))))),0)))))))</f>
@@ -15336,7 +15313,7 @@
       </c>
       <c r="S38" s="80">
         <f t="shared" ca="1" si="3"/>
-        <v>1153</v>
+        <v>0</v>
       </c>
       <c r="T38" s="65"/>
       <c r="U38" s="65"/>
@@ -16682,15 +16659,15 @@
       <c r="M59" s="233"/>
       <c r="N59" s="171">
         <f ca="1">ROUND(SUM(N35:N58),0)</f>
-        <v>4645</v>
+        <v>0</v>
       </c>
       <c r="O59" s="171">
         <f t="shared" ref="O59:S59" ca="1" si="4">SUM(O35:O58)</f>
-        <v>4977</v>
+        <v>0</v>
       </c>
       <c r="P59" s="171">
         <f t="shared" ca="1" si="4"/>
-        <v>5254</v>
+        <v>0</v>
       </c>
       <c r="Q59" s="171">
         <f t="shared" ca="1" si="4"/>
@@ -16702,7 +16679,7 @@
       </c>
       <c r="S59" s="171">
         <f t="shared" ca="1" si="4"/>
-        <v>14876</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:24">
@@ -16723,15 +16700,15 @@
       <c r="M60" s="233"/>
       <c r="N60" s="171">
         <f t="shared" ref="N60:S60" ca="1" si="5">N31+N59</f>
-        <v>84525</v>
+        <v>0</v>
       </c>
       <c r="O60" s="171">
         <f t="shared" ca="1" si="5"/>
-        <v>87254</v>
+        <v>0</v>
       </c>
       <c r="P60" s="171">
         <f t="shared" ca="1" si="5"/>
-        <v>89998</v>
+        <v>0</v>
       </c>
       <c r="Q60" s="171">
         <f t="shared" ca="1" si="5"/>
@@ -16743,7 +16720,7 @@
       </c>
       <c r="S60" s="171">
         <f t="shared" ca="1" si="5"/>
-        <v>261777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:24">
@@ -17065,7 +17042,7 @@
     <row r="75" spans="1:19">
       <c r="A75" s="161"/>
       <c r="B75" s="68" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C75" s="68"/>
       <c r="D75" s="68"/>
@@ -17078,24 +17055,28 @@
       <c r="K75" s="68"/>
       <c r="L75" s="68"/>
       <c r="M75" s="58" t="s">
-        <v>188</v>
-      </c>
-      <c r="N75" s="152"/>
+        <v>177</v>
+      </c>
+      <c r="N75" s="152">
+        <v>1400</v>
+      </c>
       <c r="O75" s="152">
-        <v>4400</v>
-      </c>
-      <c r="P75" s="152"/>
+        <v>1400</v>
+      </c>
+      <c r="P75" s="152">
+        <v>1400</v>
+      </c>
       <c r="Q75" s="152"/>
       <c r="R75" s="152"/>
       <c r="S75" s="151">
         <f>SUM(N75:R75)</f>
-        <v>4400</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="76" spans="1:19">
       <c r="A76" s="161"/>
       <c r="B76" s="68" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C76" s="68"/>
       <c r="D76" s="68"/>
@@ -17111,26 +17092,24 @@
         <v>177</v>
       </c>
       <c r="N76" s="152">
-        <v>2800</v>
+        <v>1250</v>
       </c>
       <c r="O76" s="152">
-        <v>2800</v>
+        <v>1250</v>
       </c>
       <c r="P76" s="152">
-        <v>2800</v>
+        <v>1250</v>
       </c>
       <c r="Q76" s="152"/>
       <c r="R76" s="152"/>
       <c r="S76" s="151">
         <f t="shared" ref="S76:S83" si="10">SUM(N76:R76)</f>
-        <v>8400</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="77" spans="1:19">
       <c r="A77" s="161"/>
-      <c r="B77" s="68" t="s">
-        <v>197</v>
-      </c>
+      <c r="B77" s="68"/>
       <c r="C77" s="68"/>
       <c r="D77" s="68"/>
       <c r="E77" s="68"/>
@@ -17146,14 +17125,12 @@
       </c>
       <c r="N77" s="152"/>
       <c r="O77" s="152"/>
-      <c r="P77" s="152">
-        <v>2300</v>
-      </c>
+      <c r="P77" s="152"/>
       <c r="Q77" s="152"/>
       <c r="R77" s="152"/>
       <c r="S77" s="151">
         <f t="shared" si="10"/>
-        <v>2300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:19" hidden="1">
@@ -17318,15 +17295,15 @@
       <c r="M84" s="66"/>
       <c r="N84" s="154">
         <f>SUM(N75:N83)</f>
-        <v>2800</v>
+        <v>2650</v>
       </c>
       <c r="O84" s="154">
         <f t="shared" ref="O84" si="11">SUM(O75:O83)</f>
-        <v>7200</v>
+        <v>2650</v>
       </c>
       <c r="P84" s="154">
         <f t="shared" ref="P84" si="12">SUM(P75:P83)</f>
-        <v>5100</v>
+        <v>2650</v>
       </c>
       <c r="Q84" s="154">
         <f t="shared" ref="Q84" si="13">SUM(Q75:Q83)</f>
@@ -17338,7 +17315,7 @@
       </c>
       <c r="S84" s="154">
         <f>SUM(S75:S83)</f>
-        <v>15100</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -17369,9 +17346,7 @@
     </row>
     <row r="87" spans="1:19">
       <c r="A87" s="161"/>
-      <c r="B87" s="68" t="s">
-        <v>193</v>
-      </c>
+      <c r="B87" s="68"/>
       <c r="C87" s="68"/>
       <c r="D87" s="68"/>
       <c r="E87" s="68"/>
@@ -17383,16 +17358,14 @@
       <c r="K87" s="68"/>
       <c r="L87" s="68"/>
       <c r="M87" s="68"/>
-      <c r="N87" s="80">
-        <v>3550</v>
-      </c>
+      <c r="N87" s="80"/>
       <c r="O87" s="80"/>
       <c r="P87" s="80"/>
       <c r="Q87" s="80"/>
       <c r="R87" s="80"/>
       <c r="S87" s="151">
         <f>SUM(N87:R87)</f>
-        <v>3550</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:19">
@@ -17605,7 +17578,7 @@
       <c r="M96" s="66"/>
       <c r="N96" s="154">
         <f>SUM(N87:N95)</f>
-        <v>3550</v>
+        <v>0</v>
       </c>
       <c r="O96" s="154">
         <f t="shared" ref="O96" si="17">SUM(O87:O95)</f>
@@ -17625,7 +17598,7 @@
       </c>
       <c r="S96" s="154">
         <f>SUM(S87:S95)</f>
-        <v>3550</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:19" hidden="1">
@@ -18506,15 +18479,15 @@
       </c>
       <c r="N131" s="170">
         <f ca="1">SUM(N132:N134)</f>
-        <v>13646</v>
+        <v>0</v>
       </c>
       <c r="O131" s="170">
         <f t="shared" ref="O131:R131" ca="1" si="34">SUM(O132:O134)</f>
-        <v>15010.6</v>
+        <v>0</v>
       </c>
       <c r="P131" s="170">
         <f t="shared" ca="1" si="34"/>
-        <v>16511.66</v>
+        <v>0</v>
       </c>
       <c r="Q131" s="170">
         <f t="shared" ca="1" si="34"/>
@@ -18526,7 +18499,7 @@
       </c>
       <c r="S131" s="157">
         <f ca="1">SUM(N131:R131)</f>
-        <v>45168.259999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:20">
@@ -18554,13 +18527,13 @@
       <c r="L132" s="60"/>
       <c r="M132" s="60"/>
       <c r="N132" s="80">
-        <v>13646</v>
+        <v>0</v>
       </c>
       <c r="O132" s="80">
-        <v>15010.6</v>
+        <v>0</v>
       </c>
       <c r="P132" s="80">
-        <v>16511.66</v>
+        <v>0</v>
       </c>
       <c r="Q132" s="80">
         <f ca="1">IF(AND($D$132="YES",$F$132="PY"),ROUND($G132*0.75*L132*((1+E132)^3)/9*(Worksheet!F27+Worksheet!F28),0),(IF(AND($D$132="NO",$F$132="PY"),ROUND($G132*L132*((1+E132)^3)/9*(Worksheet!F27+Worksheet!F28),0),Worksheet!H165)))</f>
@@ -18572,7 +18545,7 @@
       </c>
       <c r="S132" s="80">
         <f ca="1">SUM(N132:R132)</f>
-        <v>45168.259999999995</v>
+        <v>0</v>
       </c>
       <c r="T132" s="59"/>
     </row>
@@ -19261,15 +19234,15 @@
       <c r="M159" s="71"/>
       <c r="N159" s="158">
         <f ca="1">SUM(N132:N158)</f>
-        <v>13646</v>
+        <v>0</v>
       </c>
       <c r="O159" s="158">
         <f t="shared" ref="O159:R159" ca="1" si="38">SUM(O132:O158)</f>
-        <v>15010.6</v>
+        <v>0</v>
       </c>
       <c r="P159" s="158">
         <f t="shared" ca="1" si="38"/>
-        <v>16511.66</v>
+        <v>0</v>
       </c>
       <c r="Q159" s="158">
         <f t="shared" ca="1" si="38"/>
@@ -19281,7 +19254,7 @@
       </c>
       <c r="S159" s="171">
         <f t="shared" ca="1" si="37"/>
-        <v>45168.259999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:19">
@@ -19302,15 +19275,15 @@
       <c r="M161" s="71"/>
       <c r="N161" s="78">
         <f ca="1">N60+N72+N84+N96+N114+N126+N159</f>
-        <v>104521</v>
+        <v>2650</v>
       </c>
       <c r="O161" s="78">
         <f t="shared" ref="O161:R161" ca="1" si="39">O60+O72+O84+O96+O114+O126+O159</f>
-        <v>109464.6</v>
+        <v>2650</v>
       </c>
       <c r="P161" s="78">
         <f t="shared" ca="1" si="39"/>
-        <v>111609.66</v>
+        <v>2650</v>
       </c>
       <c r="Q161" s="78">
         <f t="shared" ca="1" si="39"/>
@@ -19322,7 +19295,7 @@
       </c>
       <c r="S161" s="78">
         <f ca="1">SUM(N161:R161)</f>
-        <v>325595.26</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="162" spans="1:19">
@@ -19347,15 +19320,15 @@
       <c r="M162" s="263"/>
       <c r="N162" s="80">
         <f ca="1">IF($H$164&lt;&gt;"Custom",(IF(F162&lt;&gt;Worksheet!A91,Worksheet!C157,IF(Request!H164="MTDC",Worksheet!C157,IF(Request!H164="TDC",Worksheet!C158,IF(Request!H164="TC",Worksheet!C159))))),0)</f>
-        <v>90875</v>
+        <v>2650</v>
       </c>
       <c r="O162" s="80">
         <f ca="1">IF($H$164&lt;&gt;"Custom",IF($F$162&lt;&gt;Worksheet!$A$91,Worksheet!D157,IF(Request!$H$164="MTDC",Worksheet!D157,IF(Request!$H$164="TDC",Worksheet!D158,IF(Request!$H$164="TC",Worksheet!D159)))),0)</f>
-        <v>94454</v>
+        <v>2650</v>
       </c>
       <c r="P162" s="80">
         <f ca="1">IF($H$164&lt;&gt;"Custom",IF($F$162&lt;&gt;Worksheet!$A$91,Worksheet!E157,IF(Request!$H$164="MTDC",Worksheet!E157,IF(Request!$H$164="TDC",Worksheet!E158,IF(Request!$H$164="TC",Worksheet!E159)))),0)</f>
-        <v>95098</v>
+        <v>2650</v>
       </c>
       <c r="Q162" s="80">
         <f>IF($H$164&lt;&gt;"Custom",IF($F$162&lt;&gt;Worksheet!$A$91,Worksheet!F157,IF(Request!$H$164="MTDC",Worksheet!F157,IF(Request!$H$164="TDC",Worksheet!F158,IF(Request!$H$164="TC",Worksheet!F159)))),0)</f>
@@ -19367,7 +19340,7 @@
       </c>
       <c r="S162" s="155">
         <f ca="1">SUM(N162:R162)</f>
-        <v>280427</v>
+        <v>7950</v>
       </c>
     </row>
     <row r="163" spans="1:19" hidden="1">
@@ -19422,15 +19395,15 @@
       <c r="M164" s="238"/>
       <c r="N164" s="83">
         <f ca="1">IF(Worksheet!C4="",0,(IF($H$164&lt;&gt;"Custom",(ROUND((((N162-SUM(N136:N140))/Worksheet!C5)*Worksheet!C9*Worksheet!B97)+((N162-SUM(N136:N140))/Worksheet!C5)*Worksheet!C10*Worksheet!C97+IF($I$135="Federal",(SUM(N136:N140)*Worksheet!B92),IF(Request!$I$135="Non-Federal",(SUM(Request!N136:N140)*Worksheet!B93))),0)),(ROUND((((N163-SUM(N136:N140))/Worksheet!C5)*Worksheet!C9*Worksheet!B97)+((N163-SUM(N136:N140))/Worksheet!C5)*Worksheet!C10*Worksheet!C97+IF($I$135="Federal",(SUM(N136:N140)*Worksheet!B92),IF(Request!$I$135="Non-Federal",(SUM(Request!N136:N140)*Worksheet!B93))),0)))))</f>
-        <v>51420</v>
+        <v>1499</v>
       </c>
       <c r="O164" s="83">
         <f ca="1">IF(Worksheet!D4="",0,(IF($H$164&lt;&gt;"Custom",(ROUND((((O162-SUM(O136:O140))/Worksheet!D5)*Worksheet!D9*Worksheet!D97)+((O162-SUM(O136:O140))/Worksheet!D5)*Worksheet!D10*Worksheet!E97+IF($I$135="Federal",(SUM(O136:O140)*Worksheet!C92),IF(Request!$I$135="Non-Federal",(SUM(Request!O136:O140)*Worksheet!C93))),0)),(ROUND((((O163-SUM(O136:O140))/Worksheet!D5)*Worksheet!D9*Worksheet!E97)+((O163-SUM(O136:O140))/Worksheet!D5)*Worksheet!D10*Worksheet!E97+IF($I$135="Federal",(SUM(O136:O140)*Worksheet!E92),IF(Request!$I$135="Non-Federal",(SUM(Request!O136:O140)*Worksheet!E93))),0)))))</f>
-        <v>53839</v>
+        <v>1511</v>
       </c>
       <c r="P164" s="83">
         <f ca="1">IF(Worksheet!E4="",0,(IF($H$164&lt;&gt;"Custom",(ROUND((((P162-SUM(P136:P140))/Worksheet!E5)*Worksheet!E9*Worksheet!F97)+((P162-SUM(P136:P140))/Worksheet!E5)*Worksheet!E10*Worksheet!F97+IF($I$135="Federal",(SUM(P136:P140)*Worksheet!F92),IF(Request!$I$135="Non-Federal",(SUM(Request!P136:P140)*Worksheet!F93))),0)),(ROUND((((P163-SUM(P136:P140))/Worksheet!E5)*Worksheet!E9*Worksheet!G97)+((P163-SUM(P136:P140))/Worksheet!E5)*Worksheet!E10*Worksheet!G97+IF($I$135="Federal",(SUM(P136:P140)*Worksheet!G92),IF(Request!$I$135="Non-Federal",(SUM(Request!P136:P140)*Worksheet!G93))),0)))))</f>
-        <v>54206</v>
+        <v>1511</v>
       </c>
       <c r="Q164" s="83">
         <f>IF(Worksheet!F4="",0,(IF($H$164&lt;&gt;"Custom",(ROUND((((Q162-SUM(Q136:Q140))/Worksheet!F5)*Worksheet!F9*Worksheet!H97)+((Q162-SUM(Q136:Q140))/Worksheet!F5)*Worksheet!F10*Worksheet!H97+IF($I$135="Federal",(SUM(Q136:Q140)*Worksheet!H92),IF(Request!$I$135="Non-Federal",(SUM(Request!Q136:Q140)*Worksheet!H93))),0)),(ROUND((((Q163-SUM(Q136:Q140))/Worksheet!F5)*Worksheet!F9*Worksheet!I97)+((Q163-SUM(Q136:Q140))/Worksheet!F5)*Worksheet!F10*Worksheet!I97+IF($I$135="Federal",(SUM(Q136:Q140)*Worksheet!I92),IF(Request!$I$135="Non-Federal",(SUM(Request!Q136:Q140)*Worksheet!I93))),0)))))</f>
@@ -19442,7 +19415,7 @@
       </c>
       <c r="S164" s="189">
         <f ca="1">SUM(N164:R164)</f>
-        <v>159465</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="165" spans="1:19">
@@ -19463,15 +19436,15 @@
       <c r="M165" s="85"/>
       <c r="N165" s="86">
         <f t="shared" ref="N165:S165" ca="1" si="40">N161+N164</f>
-        <v>155941</v>
+        <v>4149</v>
       </c>
       <c r="O165" s="86">
         <f t="shared" ca="1" si="40"/>
-        <v>163303.6</v>
+        <v>4161</v>
       </c>
       <c r="P165" s="86">
         <f t="shared" ca="1" si="40"/>
-        <v>165815.66</v>
+        <v>4161</v>
       </c>
       <c r="Q165" s="86">
         <f t="shared" ca="1" si="40"/>
@@ -19483,7 +19456,7 @@
       </c>
       <c r="S165" s="86">
         <f t="shared" ca="1" si="40"/>
-        <v>485060.26</v>
+        <v>12471</v>
       </c>
     </row>
     <row r="166" spans="1:19">
@@ -19965,7 +19938,7 @@
       <c r="G5" s="315"/>
       <c r="H5" s="316">
         <f ca="1">IF(AND(F5&lt;&gt;"",F5&lt;Worksheet!C3),(Request!N162-SUM(Request!N136:'Request'!N140))/Worksheet!C5*Worksheet!C6,Request!N162-SUM(Request!N136:'Request'!N140))</f>
-        <v>75729.166666666672</v>
+        <v>2208.3333333333335</v>
       </c>
       <c r="I5" s="316"/>
       <c r="J5" s="118">
@@ -19974,7 +19947,7 @@
       </c>
       <c r="K5" s="119">
         <f ca="1">ROUND(H5*J5,0)</f>
-        <v>42787</v>
+        <v>1248</v>
       </c>
       <c r="L5" s="120" t="str">
         <f>IF(Request!F162=Worksheet!A91,Request!H164,"MTDC")</f>
@@ -20002,7 +19975,7 @@
       <c r="G6" s="317"/>
       <c r="H6" s="310">
         <f ca="1">IF(F5&lt;Worksheet!C3,Request!N162-'F&amp;A Details'!H7-'F&amp;A Details'!H5,0)</f>
-        <v>15145.833333333328</v>
+        <v>441.66666666666652</v>
       </c>
       <c r="I6" s="310"/>
       <c r="J6" s="118">
@@ -20011,7 +19984,7 @@
       </c>
       <c r="K6" s="119">
         <f ca="1">IF(H6&lt;&gt;0,Request!N164-'F&amp;A Details'!K5-'F&amp;A Details'!K7,0)</f>
-        <v>8633</v>
+        <v>251</v>
       </c>
       <c r="L6" s="120" t="str">
         <f ca="1">IF(K6&lt;&gt;0,L5,"")</f>
@@ -20085,7 +20058,7 @@
       <c r="G9" s="302"/>
       <c r="H9" s="310">
         <f ca="1">IF(AND(F9&lt;&gt;"",F9&lt;Worksheet!D3),(Request!O162-SUM(Request!O136:O140))/Worksheet!D5*Worksheet!D6,Request!O162-SUM(Request!O136:O140))</f>
-        <v>94454</v>
+        <v>2650</v>
       </c>
       <c r="I9" s="310"/>
       <c r="J9" s="148">
@@ -20094,7 +20067,7 @@
       </c>
       <c r="K9" s="119">
         <f ca="1">ROUND(H9*J9,0)</f>
-        <v>53839</v>
+        <v>1511</v>
       </c>
       <c r="L9" s="120" t="str">
         <f>IF(Request!F162=Worksheet!A91,Request!H164,"MTDC")</f>
@@ -20206,7 +20179,7 @@
       <c r="G13" s="302"/>
       <c r="H13" s="303">
         <f ca="1">IF(AND(F13&lt;&gt;"",F13&lt;Worksheet!E3),(Request!P162-SUM(Request!P136:P140))/Worksheet!E5*Worksheet!E6,Request!P162-SUM(Request!P136:P140))</f>
-        <v>95098</v>
+        <v>2650</v>
       </c>
       <c r="I13" s="303"/>
       <c r="J13" s="118">
@@ -20215,7 +20188,7 @@
       </c>
       <c r="K13" s="119">
         <f ca="1">ROUND(H13*J13,0)</f>
-        <v>54206</v>
+        <v>1511</v>
       </c>
       <c r="L13" s="120" t="str">
         <f>IF(Request!F162=Worksheet!A91,Request!H164,"MTDC")</f>
@@ -20482,7 +20455,7 @@
       <c r="J22" s="301"/>
       <c r="K22" s="149">
         <f ca="1">SUM(K5:K21)</f>
-        <v>159465</v>
+        <v>4521</v>
       </c>
       <c r="L22" s="150"/>
       <c r="M22" s="144" t="b">

</xml_diff>